<commit_message>
auth updated, exel not totaly updated
</commit_message>
<xml_diff>
--- a/analysis/ASVS-checklist-en.xlsx
+++ b/analysis/ASVS-checklist-en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\CODE\UA\SIO\2nd-project-group_19\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8A23E7-D5EE-4B67-A7A5-5231205A85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D118CBA-56AE-4785-BFB8-2CFD6F68A38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="839" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="839" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="689">
   <si>
     <t>Security Category</t>
   </si>
@@ -2182,6 +2182,12 @@
   </si>
   <si>
     <t>Non-valid</t>
+  </si>
+  <si>
+    <t>A hash deixa a password do mesmo tamanho</t>
+  </si>
+  <si>
+    <t>So quando erra na pass no register(alterar para mostrar logo no inicio)</t>
   </si>
 </sst>
 </file>
@@ -3510,7 +3516,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>14.035087719298245</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3549,7 +3555,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7543859649122806</c:v>
+                  <c:v>4.5614035087719298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7050,7 +7056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -7105,7 +7111,7 @@
       </c>
       <c r="B3" s="113">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3" s="114">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -7113,7 +7119,7 @@
       </c>
       <c r="D3" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.035087719298245</v>
       </c>
       <c r="E3" s="116"/>
     </row>
@@ -7340,7 +7346,7 @@
       </c>
       <c r="B16" s="113">
         <f>SUM(B2:B15)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C16" s="114">
         <f>SUM(C2:C15)</f>
@@ -7348,7 +7354,7 @@
       </c>
       <c r="D16" s="115">
         <f t="shared" si="0"/>
-        <v>1.7543859649122806</v>
+        <v>4.5614035087719298</v>
       </c>
       <c r="E16" s="116"/>
     </row>
@@ -7368,8 +7374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -7436,7 +7442,9 @@
       <c r="F2" s="39" t="s">
         <v>580</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="40" t="s">
+        <v>16</v>
+      </c>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
       <c r="J2" s="42"/>
@@ -7458,9 +7466,13 @@
       <c r="F3" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="18" t="s">
+        <v>686</v>
+      </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="I3" s="20" t="s">
+        <v>687</v>
+      </c>
       <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -7480,9 +7492,13 @@
       <c r="F4" s="19" t="s">
         <v>582</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="18" t="s">
+        <v>686</v>
+      </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>687</v>
+      </c>
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -7502,7 +7518,9 @@
       <c r="F5" s="19" t="s">
         <v>583</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="21"/>
@@ -7524,7 +7542,9 @@
       <c r="F6" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="21"/>
@@ -7546,7 +7566,9 @@
       <c r="F7" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
       <c r="J7" s="21"/>
@@ -7573,7 +7595,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="123"/>
       <c r="B9" s="35" t="s">
         <v>127</v>
@@ -7590,9 +7612,13 @@
       <c r="F9" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="G9" s="18"/>
+      <c r="G9" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>688</v>
+      </c>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" s="15" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7612,7 +7638,9 @@
       <c r="F10" s="19" t="s">
         <v>585</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>686</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
@@ -7634,7 +7662,9 @@
       <c r="F11" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="18" t="s">
+        <v>686</v>
+      </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
@@ -7656,7 +7686,9 @@
       <c r="F12" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
@@ -8058,7 +8090,9 @@
       <c r="F30" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="G30" s="18"/>
+      <c r="G30" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
       <c r="J30" s="22"/>
@@ -8080,7 +8114,9 @@
       <c r="F31" s="19" t="s">
         <v>594</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="18" t="s">
+        <v>686</v>
+      </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="22"/>
@@ -8102,7 +8138,9 @@
       <c r="F32" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="G32" s="18"/>
+      <c r="G32" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
       <c r="J32" s="22"/>
@@ -8555,7 +8593,7 @@
       <c r="I52" s="18"/>
       <c r="J52" s="22"/>
     </row>
-    <row r="53" spans="1:10" s="15" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" s="15" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="123"/>
       <c r="B53" s="35" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Updated and data cleared from client storage
</commit_message>
<xml_diff>
--- a/analysis/ASVS-checklist-en.xlsx
+++ b/analysis/ASVS-checklist-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\CODE\UA\SIO\2nd-project-group_19\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864FF8CE-72AF-492F-B42F-222D9F82330C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0D3ADF-E16E-49BB-92E9-FC9A12581054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" tabRatio="839" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="839" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="694">
   <si>
     <t>Security Category</t>
   </si>
@@ -2197,6 +2197,12 @@
   </si>
   <si>
     <t>So quando erra na pass no register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penso que esteja valido </t>
+  </si>
+  <si>
+    <t>implementar</t>
   </si>
 </sst>
 </file>
@@ -3525,7 +3531,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.789473684210526</c:v>
+                  <c:v>16.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3543,7 +3549,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3564,7 +3570,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.9122807017543861</c:v>
+                  <c:v>5.376344086021505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4263,7 +4269,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10" s="15" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="15" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="122"/>
       <c r="B11" s="8" t="s">
         <v>51</v>
@@ -4937,17 +4943,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A43"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
@@ -4970,7 +4976,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -5037,7 +5043,9 @@
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="I2" s="40" t="s">
+        <v>693</v>
+      </c>
       <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -5206,8 +5214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -5720,7 +5728,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -5785,7 +5793,9 @@
       <c r="F2" s="70" t="s">
         <v>664</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="40" t="s">
+        <v>685</v>
+      </c>
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
       <c r="J2" s="60"/>
@@ -5869,7 +5879,9 @@
       <c r="F6" s="71" t="s">
         <v>665</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="18" t="s">
+        <v>685</v>
+      </c>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
       <c r="J6" s="22"/>
@@ -6107,7 +6119,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -6488,8 +6500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -7124,11 +7136,11 @@
       </c>
       <c r="C3" s="114">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" s="115">
         <f t="shared" si="0"/>
-        <v>15.789473684210526</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="E3" s="116"/>
     </row>
@@ -7229,15 +7241,15 @@
       </c>
       <c r="B9" s="113">
         <f>COUNTIF('Data Protection'!G2:G18,"Valid")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="114">
         <f>COUNTIF('Data Protection'!G2:G18,"&lt;&gt;Not Applicable")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="E9" s="116"/>
     </row>
@@ -7305,7 +7317,7 @@
       </c>
       <c r="C13" s="114">
         <f>COUNTIF('Files and Resources'!G2:G16,"&lt;&gt;Not Applicable")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="115">
         <f t="shared" si="0"/>
@@ -7355,15 +7367,15 @@
       </c>
       <c r="B16" s="113">
         <f>SUM(B2:B15)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="114">
         <f>SUM(C2:C15)</f>
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D16" s="115">
         <f t="shared" si="0"/>
-        <v>4.9122807017543861</v>
+        <v>5.376344086021505</v>
       </c>
       <c r="E16" s="116"/>
     </row>
@@ -7383,8 +7395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -8132,7 +8144,7 @@
         <v>594</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
@@ -8179,7 +8191,9 @@
       <c r="F33" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="G33" s="18"/>
+      <c r="G33" s="18" t="s">
+        <v>685</v>
+      </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
       <c r="J33" s="22"/>
@@ -8201,7 +8215,9 @@
       <c r="F34" s="19" t="s">
         <v>595</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="18" t="s">
+        <v>685</v>
+      </c>
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
       <c r="J34" s="22"/>
@@ -10290,7 +10306,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -10693,7 +10709,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -11034,7 +11050,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -11261,10 +11277,13 @@
       <c r="F10" s="71" t="s">
         <v>405</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="22"/>
+      <c r="I10" s="18" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="123" t="s">
@@ -11303,7 +11322,9 @@
       <c r="F12" s="71" t="s">
         <v>407</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="18" t="s">
+        <v>685</v>
+      </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="22"/>

</xml_diff>